<commit_message>
In Xlsx class add reading from *.xlsx file and checking empty fields.
</commit_message>
<xml_diff>
--- a/data/hosts.xlsx
+++ b/data/hosts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>address</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>Switch drugi</t>
+  </si>
+  <si>
+    <t>Switch glowny3</t>
+  </si>
+  <si>
+    <t>Switch glowny4</t>
+  </si>
+  <si>
+    <t>Router V5</t>
+  </si>
+  <si>
+    <t>Opisdwa</t>
+  </si>
+  <si>
+    <t>Switch glowny5</t>
   </si>
 </sst>
 </file>
@@ -408,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,16 +480,31 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -484,24 +514,6 @@
       </c>
       <c r="D3">
         <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -538,33 +550,18 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -598,6 +595,48 @@
       </c>
       <c r="K7" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import host from *.xlsx file to sqlite is working!
</commit_message>
<xml_diff>
--- a/data/hosts.xlsx
+++ b/data/hosts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>address</t>
   </si>
@@ -45,9 +45,6 @@
     <t>192.168.1.5</t>
   </si>
   <si>
-    <t>Switch glowny</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -93,19 +90,13 @@
     <t>Switch drugi</t>
   </si>
   <si>
-    <t>Switch glowny3</t>
-  </si>
-  <si>
     <t>Switch glowny4</t>
   </si>
   <si>
-    <t>Router V5</t>
-  </si>
-  <si>
     <t>Opisdwa</t>
   </si>
   <si>
-    <t>Switch glowny5</t>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -423,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,34 +431,34 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -475,7 +466,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -484,19 +475,19 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
         <v>6</v>
@@ -504,16 +495,34 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3">
         <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -521,122 +530,16 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
With category in database
</commit_message>
<xml_diff>
--- a/data/hosts.xlsx
+++ b/data/hosts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -103,7 +103,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,128 +425,129 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="1" max="11" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A lot of changes. Added service table.
</commit_message>
<xml_diff>
--- a/data/hosts.xlsx
+++ b/data/hosts.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Routers" sheetId="1" r:id="rId1"/>
+    <sheet name="Switches" sheetId="3" r:id="rId2"/>
+    <sheet name="Services" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>address</t>
   </si>
@@ -97,13 +99,72 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>fa0/1</t>
+  </si>
+  <si>
+    <t>192.168.1.6</t>
+  </si>
+  <si>
+    <t>Routers</t>
+  </si>
+  <si>
+    <t>Switches</t>
+  </si>
+  <si>
+    <t>Router V2</t>
+  </si>
+  <si>
+    <t>Opis asdasd</t>
+  </si>
+  <si>
+    <t>192.168.1.2</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>uptime</t>
+  </si>
+  <si>
+    <t>ping</t>
+  </si>
+  <si>
+    <t>interface_status</t>
+  </si>
+  <si>
+    <t>interface_utilization</t>
+  </si>
+  <si>
+    <t>chassis_temperature</t>
+  </si>
+  <si>
+    <t>fan_status</t>
+  </si>
+  <si>
+    <t>fa0/3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,9 +200,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,17 +485,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="11" width="15.85546875" style="2" customWidth="1"/>
+    <col min="12" max="15" width="14.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749D4821-11C9-4822-B16D-C4CF8FDC5CFB}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -472,17 +652,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
       </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
@@ -499,59 +680,115 @@
         <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565D5039-A34D-4B72-993A-4F7C6A4CFDE1}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="11.5703125" style="3" customWidth="1"/>
+    <col min="4" max="6" width="21.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Before to add column for each services in datatabse.
</commit_message>
<xml_diff>
--- a/data/hosts.xlsx
+++ b/data/hosts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Routers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>address</t>
   </si>
@@ -31,9 +31,6 @@
     <t>community</t>
   </si>
   <si>
-    <t>192.168.1.1</t>
-  </si>
-  <si>
     <t>Router V1</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>authPriv</t>
-  </si>
-  <si>
     <t>DES</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t>ok</t>
   </si>
   <si>
-    <t>fa0/1</t>
-  </si>
-  <si>
     <t>192.168.1.6</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>Opis asdasd</t>
   </si>
   <si>
-    <t>192.168.1.2</t>
-  </si>
-  <si>
     <t>uptime</t>
   </si>
   <si>
@@ -133,19 +121,19 @@
     <t>fa0/3</t>
   </si>
   <si>
-    <t>werwer</t>
-  </si>
-  <si>
-    <t>wrewre</t>
-  </si>
-  <si>
-    <t>rewer</t>
-  </si>
-  <si>
     <t>sss</t>
   </si>
   <si>
     <t>aaaa</t>
+  </si>
+  <si>
+    <t>FastEthernet0/0</t>
+  </si>
+  <si>
+    <t>FastEthernet0/0, FastEthernet0/1</t>
+  </si>
+  <si>
+    <t>192.168.202.1</t>
   </si>
 </sst>
 </file>
@@ -490,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,146 +494,125 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D2" s="3">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="L2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>35</v>
+      </c>
+      <c r="O2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D3" s="3">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4"/>
       <c r="L3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="M3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>25</v>
+      <c r="N3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -658,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749D4821-11C9-4822-B16D-C4CF8FDC5CFB}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,85 +639,85 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L2" s="2" t="b">
         <v>1</v>
@@ -759,10 +726,10 @@
         <v>1</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="P2" s="2" t="b">
         <v>1</v>
@@ -773,19 +740,19 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -800,10 +767,10 @@
         <v>1</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="P3" s="2" t="b">
         <v>1</v>
@@ -814,5 +781,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>